<commit_message>
update matlabscript and filedescription
</commit_message>
<xml_diff>
--- a/file_description.xlsx
+++ b/file_description.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E92482-01DC-1240-82C3-F462C1C0DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333A36C5-17EB-BA4B-842C-F4607ADC004F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code_spec" sheetId="4" r:id="rId1"/>
     <sheet name="matlab_script" sheetId="6" r:id="rId2"/>
     <sheet name="Config_spec" sheetId="2" r:id="rId3"/>
     <sheet name="Data_spec" sheetId="5" r:id="rId4"/>
+    <sheet name="BrainNetViewer_colormap" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="302">
   <si>
     <t>Name</t>
   </si>
@@ -808,6 +809,138 @@
   </si>
   <si>
     <t>SCORE NAME corresponds to variable name, see cognitive measure csv. Not sure where these are cleaned from, maybe add_cog,ipynb</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>pt12_vi.mat</t>
+  </si>
+  <si>
+    <t>amy_d2blest_pos.mat</t>
+  </si>
+  <si>
+    <t>mri_d2blest_pt25.mat</t>
+  </si>
+  <si>
+    <t>*txt</t>
+  </si>
+  <si>
+    <t>colormap matrix to be imported into the custom colormap option in brainnet viewer's configuration menu</t>
+  </si>
+  <si>
+    <t>generate the double threshold time from baseline slope map from voxelstat output</t>
+  </si>
+  <si>
+    <t>individual.m</t>
+  </si>
+  <si>
+    <t>day2bl_double_p_combo.m</t>
+  </si>
+  <si>
+    <t>visualize SUVR images for all the Flortaucipir PET in this project</t>
+  </si>
+  <si>
+    <t>poorly.m</t>
+  </si>
+  <si>
+    <t>create and visualize the average Flortaucipir PET SUVR images of the group of participants with poor model fit in solutions with different number of subtypes</t>
+  </si>
+  <si>
+    <t>cmap_generator.m</t>
+  </si>
+  <si>
+    <t>matlab version of colormap generator for brainnetviewer</t>
+  </si>
+  <si>
+    <t>outdated (kinda)</t>
+  </si>
+  <si>
+    <t>vs_script</t>
+  </si>
+  <si>
+    <t>run voxelstat using matlab script instead of the GUI to save and visualize output more efficiently</t>
+  </si>
+  <si>
+    <t>run_vs_script</t>
+  </si>
+  <si>
+    <t>batch_vs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function to run voxelstat with self-defined input output and parameters + visualization </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch run (call run_vs_script) to set a list of LME modeling to run + </t>
+  </si>
+  <si>
+    <t>tmap_afni.mat</t>
+  </si>
+  <si>
+    <t>flexible_doublep_baselinecomp</t>
+  </si>
+  <si>
+    <t>baseline_subtype_ss_avg</t>
+  </si>
+  <si>
+    <t>generate and visualize subtype and subtype-stage group average Flortaucipir PET SUVR images</t>
+  </si>
+  <si>
+    <t>TPM_GM_Mask_10pc.nii</t>
+  </si>
+  <si>
+    <t>Grey matter mask derived from SPM</t>
+  </si>
+  <si>
+    <t>rs16Sub_harbard_bin01.nii</t>
+  </si>
+  <si>
+    <t>the balue is inverse</t>
+  </si>
+  <si>
+    <t>cet_rbgyrm1_pt5_3.mat</t>
+  </si>
+  <si>
+    <t>combined_darkred.mat</t>
+  </si>
+  <si>
+    <t>binary colormap for anova test in LME</t>
+  </si>
+  <si>
+    <t>pt5_3pt5_magma_shifted_stage.mat</t>
+  </si>
+  <si>
+    <t>doublep_thre3</t>
+  </si>
+  <si>
+    <t>baseline comparison with different covariate adjustment, modalities, and number of subtypes</t>
+  </si>
+  <si>
+    <t>onevr_double_p_combo.m</t>
+  </si>
+  <si>
+    <t>visualize comparison result (after running flexible doublep and get combined contrast nifti for adjusted and unadjusted) using double significance threshold</t>
+  </si>
+  <si>
+    <t>baseline subtype-versus-rest comparison t value map with double significance threshold</t>
+  </si>
+  <si>
+    <t>subtype and stage group average Flortaucipir PET SUVR images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope (year_to_baseline) map for T1-weighted MRI LME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope (year_to_baseline) map for Florbetaben PET LME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">slope (year_to_baseline) map for Flortaucipir PET LME </t>
+  </si>
+  <si>
+    <t>t-value maps (after they've been filtered out based on significance threshold)</t>
+  </si>
+  <si>
+    <t>rainbow colormap for average Flortaucipir SUVR maps (alternative: lm_inferno)</t>
   </si>
 </sst>
 </file>
@@ -882,7 +1015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -908,7 +1041,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1642,13 +1774,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912AD624-BB75-3743-A749-677D732C4CEA}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -1659,6 +1795,105 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A12" sqref="A12"/>
     </sheetView>
@@ -2148,7 +2383,6 @@
       <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -2453,4 +2687,103 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D640457-302C-8442-BA2F-E9D6744A91DD}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="219" zoomScaleNormal="219" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>